<commit_message>
Added new datasheets, updated register document.
</commit_message>
<xml_diff>
--- a/datasheets/8-bit register details.xlsx
+++ b/datasheets/8-bit register details.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\YABEIC\datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8BD1565-90CF-4910-A7F0-8236639D2AA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0720095C-55AB-40D5-8BC6-BA0D477D918B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{F89BBC80-92E9-444B-9BBB-0FBCC14392D4}"/>
   </bookViews>
@@ -415,7 +415,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,7 +459,7 @@
       <c r="A3">
         <v>373</v>
       </c>
-      <c r="E3" t="s">
+      <c r="D3" t="s">
         <v>5</v>
       </c>
       <c r="F3" t="s">

</xml_diff>